<commit_message>
add graph of leaf, add graphs to slides
</commit_message>
<xml_diff>
--- a/Spectra.graphs.xlsx
+++ b/Spectra.graphs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lizzie\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lizzie\MoonSpectroscopy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -254,10 +254,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="3.1502352528514577E-2"/>
+          <c:x val="3.99508932351198E-2"/>
           <c:y val="1.1317559185698803E-2"/>
-          <c:w val="0.83476356555973985"/>
-          <c:h val="0.94675049505287012"/>
+          <c:w val="0.82631499691570798"/>
+          <c:h val="0.92288413232355515"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1860,11 +1860,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="343866136"/>
-        <c:axId val="343867704"/>
+        <c:axId val="292674808"/>
+        <c:axId val="292678368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="343866136"/>
+        <c:axId val="292674808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="950"/>
@@ -1872,28 +1872,72 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Wavelength/</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t>nm</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="343867704"/>
+        <c:crossAx val="292678368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="343867704"/>
+        <c:axId val="292678368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Intensity/AU</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="343866136"/>
+        <c:crossAx val="292674808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3273,12 +3317,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="343868488"/>
-        <c:axId val="343870840"/>
-        <c:axId val="346607208"/>
+        <c:axId val="292677584"/>
+        <c:axId val="292678760"/>
+        <c:axId val="292716088"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="343868488"/>
+        <c:axId val="292677584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3315,7 +3359,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343870840"/>
+        <c:crossAx val="292678760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3323,7 +3367,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="343870840"/>
+        <c:axId val="292678760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3374,12 +3418,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343868488"/>
+        <c:crossAx val="292677584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="346607208"/>
+        <c:axId val="292716088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3415,7 +3459,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343870840"/>
+        <c:crossAx val="292678760"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
       <c:spPr>
@@ -3511,6 +3555,261 @@
     <c:title>
       <c:layout/>
       <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.1502352528514577E-2"/>
+          <c:y val="1.1317559185698803E-2"/>
+          <c:w val="0.83476356555973985"/>
+          <c:h val="0.94675049505287012"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Leaf:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$19:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>555</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>585</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>605</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>635</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>695</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>880</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>940</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>249</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>412</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>615</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>405</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="295625168"/>
+        <c:axId val="295626344"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="295625168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="950"/>
+          <c:min val="450"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="295626344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="295626344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="295625168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="5000"/>
+                <a:lumOff val="95000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="76000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="45000"/>
+                <a:lumOff val="55000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="94000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="45000"/>
+                <a:lumOff val="55000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="30000"/>
+                <a:lumOff val="70000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.87188363003537606"/>
+          <c:y val="0.17476768344713525"/>
+          <c:w val="0.12449318155882688"/>
+          <c:h val="0.44982371606534249"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -4825,11 +5124,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="343866920"/>
-        <c:axId val="343867312"/>
+        <c:axId val="292677976"/>
+        <c:axId val="292675232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="343866920"/>
+        <c:axId val="292677976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -4888,12 +5187,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343867312"/>
+        <c:crossAx val="292675232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="343867312"/>
+        <c:axId val="292675232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -4951,7 +5250,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343866920"/>
+        <c:crossAx val="292677976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6143,8 +6442,8 @@
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6188,6 +6487,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6520,8 +6851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:B24"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="N129" sqref="N129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
edit excel graphs to %
</commit_message>
<xml_diff>
--- a/Spectra.graphs.xlsx
+++ b/Spectra.graphs.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -268,7 +268,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$18</c:f>
+              <c:f>Sheet1!$N$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -290,7 +290,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$27</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -326,36 +326,36 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$19:$G$27</c:f>
+              <c:f>Sheet1!$N$19:$N$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>240</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>278</c:v>
+                  <c:v>13.900000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>258</c:v>
+                  <c:v>12.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>259</c:v>
+                  <c:v>12.950000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>250</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>280</c:v>
+                  <c:v>14.000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>300</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>280</c:v>
+                  <c:v>14.000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>215</c:v>
+                  <c:v>10.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -367,7 +367,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$18</c:f>
+              <c:f>Sheet1!$Z$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -397,7 +397,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$27</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -433,36 +433,36 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$M$19:$M$27</c:f>
+              <c:f>Sheet1!$Z$19:$Z$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>260</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>145</c:v>
+                  <c:v>7.2499999999999991</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>138</c:v>
+                  <c:v>6.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>130</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>128</c:v>
+                  <c:v>6.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>213</c:v>
+                  <c:v>10.65</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>209</c:v>
+                  <c:v>10.45</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>524</c:v>
+                  <c:v>26.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>354</c:v>
+                  <c:v>17.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -474,7 +474,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$18</c:f>
+              <c:f>Sheet1!$X$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -504,7 +504,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$27</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -540,36 +540,36 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$L$19:$L$27</c:f>
+              <c:f>Sheet1!$X$19:$X$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>163</c:v>
+                  <c:v>8.15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>252</c:v>
+                  <c:v>12.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>165</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>137</c:v>
+                  <c:v>6.8500000000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>133</c:v>
+                  <c:v>6.65</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>181</c:v>
+                  <c:v>9.0499999999999989</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>189</c:v>
+                  <c:v>9.4499999999999993</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>369</c:v>
+                  <c:v>18.45</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256</c:v>
+                  <c:v>12.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -581,7 +581,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$18</c:f>
+              <c:f>Sheet1!$E$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -612,7 +612,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$27</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -648,36 +648,36 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:f>Sheet1!$E$19:$E$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>151</c:v>
+                  <c:v>7.55</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>280</c:v>
+                  <c:v>14.000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>211</c:v>
+                  <c:v>10.549999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>165</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>123</c:v>
+                  <c:v>6.15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>249</c:v>
+                  <c:v>12.45</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>412</c:v>
+                  <c:v>20.599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>615</c:v>
+                  <c:v>30.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>405</c:v>
+                  <c:v>20.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -689,7 +689,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$18</c:f>
+              <c:f>Sheet1!$AB$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -719,7 +719,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$27</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -755,36 +755,36 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$19:$N$27</c:f>
+              <c:f>Sheet1!$AB$19:$AB$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>355</c:v>
+                  <c:v>17.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>690</c:v>
+                  <c:v>34.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>463</c:v>
+                  <c:v>23.150000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>385</c:v>
+                  <c:v>19.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>367</c:v>
+                  <c:v>18.350000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>510</c:v>
+                  <c:v>25.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>634</c:v>
+                  <c:v>31.7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>900</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>577</c:v>
+                  <c:v>28.849999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -796,7 +796,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Q$18</c:f>
+              <c:f>Sheet1!$AH$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -826,7 +826,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$27</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -862,36 +862,36 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$19:$Q$27</c:f>
+              <c:f>Sheet1!$AH$19:$AH$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>393</c:v>
+                  <c:v>19.650000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1221</c:v>
+                  <c:v>61.050000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1219</c:v>
+                  <c:v>60.95</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1134</c:v>
+                  <c:v>56.699999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1119</c:v>
+                  <c:v>55.95</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1250</c:v>
+                  <c:v>62.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1353</c:v>
+                  <c:v>67.650000000000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1195</c:v>
+                  <c:v>59.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>692</c:v>
+                  <c:v>34.599999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -903,7 +903,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$18</c:f>
+              <c:f>Sheet1!$AD$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -933,7 +933,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$27</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -969,36 +969,36 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$O$19:$O$27</c:f>
+              <c:f>Sheet1!$AD$19:$AD$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>387</c:v>
+                  <c:v>19.350000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1242</c:v>
+                  <c:v>62.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1222</c:v>
+                  <c:v>61.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1104</c:v>
+                  <c:v>55.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1084</c:v>
+                  <c:v>54.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1199</c:v>
+                  <c:v>59.95</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1271</c:v>
+                  <c:v>63.55</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1050</c:v>
+                  <c:v>52.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>644</c:v>
+                  <c:v>32.200000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1010,7 +1010,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$18</c:f>
+              <c:f>Sheet1!$AF$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1040,7 +1040,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$27</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1076,36 +1076,36 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$P$19:$P$27</c:f>
+              <c:f>Sheet1!$AF$19:$AF$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>211</c:v>
+                  <c:v>10.549999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>234</c:v>
+                  <c:v>11.700000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>374</c:v>
+                  <c:v>18.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>520</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>602</c:v>
+                  <c:v>30.099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>719</c:v>
+                  <c:v>35.949999999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>804</c:v>
+                  <c:v>40.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>765</c:v>
+                  <c:v>38.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>465</c:v>
+                  <c:v>23.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1117,7 +1117,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$18</c:f>
+              <c:f>Sheet1!$R$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1147,7 +1147,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$27</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1183,36 +1183,36 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$19:$I$27</c:f>
+              <c:f>Sheet1!$R$19:$R$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>331</c:v>
+                  <c:v>16.55</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>550</c:v>
+                  <c:v>27.500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>575</c:v>
+                  <c:v>28.749999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>532</c:v>
+                  <c:v>26.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>510</c:v>
+                  <c:v>25.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>608</c:v>
+                  <c:v>30.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>72</c:v>
+                  <c:v>3.5999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>623</c:v>
+                  <c:v>31.15</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>395</c:v>
+                  <c:v>19.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1224,7 +1224,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$18</c:f>
+              <c:f>Sheet1!$T$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1254,7 +1254,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$27</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1290,36 +1290,36 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$19:$J$27</c:f>
+              <c:f>Sheet1!$T$19:$T$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>198</c:v>
+                  <c:v>9.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>252</c:v>
+                  <c:v>12.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>230</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>147</c:v>
+                  <c:v>7.35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>227</c:v>
+                  <c:v>11.35</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>253</c:v>
+                  <c:v>12.65</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>247</c:v>
+                  <c:v>12.35</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>190</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>140</c:v>
+                  <c:v>7.0000000000000009</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1331,7 +1331,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$18</c:f>
+              <c:f>Sheet1!$G$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1361,7 +1361,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$27</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1397,36 +1397,36 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$19:$D$27</c:f>
+              <c:f>Sheet1!$G$19:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>266</c:v>
+                  <c:v>13.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>353</c:v>
+                  <c:v>17.649999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>321</c:v>
+                  <c:v>16.05</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>256</c:v>
+                  <c:v>12.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>225</c:v>
+                  <c:v>11.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>271</c:v>
+                  <c:v>13.55</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>279</c:v>
+                  <c:v>13.950000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>220</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>158</c:v>
+                  <c:v>7.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1438,7 +1438,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$18</c:f>
+              <c:f>Sheet1!$P$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1470,7 +1470,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$27</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1506,36 +1506,36 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$19:$H$27</c:f>
+              <c:f>Sheet1!$P$19:$P$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1056</c:v>
+                  <c:v>52.800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1125</c:v>
+                  <c:v>56.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1030</c:v>
+                  <c:v>51.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1017</c:v>
+                  <c:v>50.849999999999994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>983</c:v>
+                  <c:v>49.15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1075</c:v>
+                  <c:v>53.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1200</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1040</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>593</c:v>
+                  <c:v>29.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1547,7 +1547,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$18</c:f>
+              <c:f>Sheet1!$I$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1581,7 +1581,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$27</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1617,30 +1617,30 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$19:$E$27</c:f>
+              <c:f>Sheet1!$I$19:$I$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="1">
-                  <c:v>1950</c:v>
+                  <c:v>97.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>816</c:v>
+                  <c:v>40.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>630</c:v>
+                  <c:v>31.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>711</c:v>
+                  <c:v>35.549999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>930</c:v>
+                  <c:v>46.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1360</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1233</c:v>
+                  <c:v>61.650000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1652,7 +1652,7 @@
           <c:order val="13"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$18</c:f>
+              <c:f>Sheet1!$L$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1685,7 +1685,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$27</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1721,24 +1721,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$19:$F$27</c:f>
+              <c:f>Sheet1!$L$19:$L$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="2">
-                  <c:v>1421</c:v>
+                  <c:v>71.05</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1695</c:v>
+                  <c:v>84.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1299</c:v>
+                  <c:v>64.95</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1415</c:v>
+                  <c:v>70.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1160</c:v>
+                  <c:v>57.999999999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1750,7 +1750,7 @@
           <c:order val="14"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$18</c:f>
+              <c:f>Sheet1!$V$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1780,7 +1780,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$27</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1816,36 +1816,36 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$K$19:$K$27</c:f>
+              <c:f>Sheet1!$V$19:$V$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>125</c:v>
+                  <c:v>6.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>152</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>157</c:v>
+                  <c:v>7.85</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>137</c:v>
+                  <c:v>6.8500000000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>141</c:v>
+                  <c:v>7.0499999999999989</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>262</c:v>
+                  <c:v>13.100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>497</c:v>
+                  <c:v>24.85</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>725</c:v>
+                  <c:v>36.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>460</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1860,11 +1860,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="292674808"/>
-        <c:axId val="292678368"/>
+        <c:axId val="296490040"/>
+        <c:axId val="296522408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="292674808"/>
+        <c:axId val="296490040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="950"/>
@@ -1900,16 +1900,15 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="292678368"/>
+        <c:crossAx val="296522408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="292678368"/>
+        <c:axId val="296522408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="2000"/>
-          <c:min val="0"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1937,7 +1936,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="292674808"/>
+        <c:crossAx val="296490040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2025,6 +2024,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2105,7 +2105,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2180,7 +2180,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$16</c:f>
+              <c:f>Sheet1!$E$2:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2238,7 +2238,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2313,7 +2313,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$16</c:f>
+              <c:f>Sheet1!$G$2:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2371,7 +2371,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>Sheet1!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2446,7 +2446,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$16</c:f>
+              <c:f>Sheet1!$I$2:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2504,7 +2504,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>Sheet1!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2582,7 +2582,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$16</c:f>
+              <c:f>Sheet1!$L$2:$L$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2640,7 +2640,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>Sheet1!$N$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2717,7 +2717,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$16</c:f>
+              <c:f>Sheet1!$N$2:$N$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2775,7 +2775,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>Sheet1!$P$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2850,7 +2850,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$16</c:f>
+              <c:f>Sheet1!$P$2:$P$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2908,7 +2908,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$1</c:f>
+              <c:f>Sheet1!$R$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2983,7 +2983,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$16</c:f>
+              <c:f>Sheet1!$R$2:$R$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -3041,7 +3041,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$1</c:f>
+              <c:f>Sheet1!$T$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3118,7 +3118,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$16</c:f>
+              <c:f>Sheet1!$T$2:$T$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -3176,7 +3176,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$1</c:f>
+              <c:f>Sheet1!$V$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3254,7 +3254,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$16</c:f>
+              <c:f>Sheet1!$V$2:$V$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -3317,12 +3317,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="292677584"/>
-        <c:axId val="292678760"/>
-        <c:axId val="292716088"/>
+        <c:axId val="296521624"/>
+        <c:axId val="296522016"/>
+        <c:axId val="297141280"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="292677584"/>
+        <c:axId val="296521624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3359,7 +3359,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="292678760"/>
+        <c:crossAx val="296522016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3367,7 +3367,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="292678760"/>
+        <c:axId val="296522016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3418,12 +3418,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="292677584"/>
+        <c:crossAx val="296521624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="292716088"/>
+        <c:axId val="297141280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3459,7 +3459,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="292678760"/>
+        <c:crossAx val="296522016"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
       <c:spPr>
@@ -3472,6 +3472,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3577,7 +3578,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$18</c:f>
+              <c:f>Sheet1!$E$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3608,7 +3609,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$27</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -3644,36 +3645,36 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:f>Sheet1!$E$19:$E$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>151</c:v>
+                  <c:v>7.55</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>280</c:v>
+                  <c:v>14.000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>211</c:v>
+                  <c:v>10.549999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>165</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>123</c:v>
+                  <c:v>6.15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>249</c:v>
+                  <c:v>12.45</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>412</c:v>
+                  <c:v>20.599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>615</c:v>
+                  <c:v>30.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>405</c:v>
+                  <c:v>20.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3688,11 +3689,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="295625168"/>
-        <c:axId val="295626344"/>
+        <c:axId val="296524760"/>
+        <c:axId val="296523584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="295625168"/>
+        <c:axId val="296524760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="950"/>
@@ -3704,12 +3705,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="295626344"/>
+        <c:crossAx val="296523584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="295626344"/>
+        <c:axId val="296523584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -3721,7 +3722,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="295625168"/>
+        <c:crossAx val="296524760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5124,11 +5125,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="292677976"/>
-        <c:axId val="292675232"/>
+        <c:axId val="296523192"/>
+        <c:axId val="296523976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="292677976"/>
+        <c:axId val="296523192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -5187,12 +5188,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="292675232"/>
+        <c:crossAx val="296523976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="292675232"/>
+        <c:axId val="296523976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -5250,7 +5251,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="292677976"/>
+        <c:crossAx val="296523192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6440,7 +6441,7 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>39</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>71</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -6464,13 +6465,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>31</xdr:col>
+      <xdr:col>48</xdr:col>
       <xdr:colOff>609599</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>49</xdr:col>
+      <xdr:col>66</xdr:col>
       <xdr:colOff>295274</xdr:colOff>
       <xdr:row>63</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
@@ -6500,7 +6501,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>39</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>112</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -6849,1054 +6850,1800 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S27"/>
+  <dimension ref="A1:AJ27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="N129" sqref="N129"/>
+    <sheetView tabSelected="1" topLeftCell="P79" workbookViewId="0">
+      <selection activeCell="AH19" sqref="AH19:AH27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="32.5703125" customWidth="1"/>
+    <col min="1" max="4" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C1" s="11" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="11"/>
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
+      <c r="N1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
+      <c r="P1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
+      <c r="R1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" t="s">
+      <c r="T1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" t="s">
+      <c r="V1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="2">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2">
         <v>151</v>
       </c>
-      <c r="D2" s="4">
+      <c r="F2" s="2"/>
+      <c r="G2" s="4">
         <v>280</v>
       </c>
-      <c r="E2" s="3">
+      <c r="H2" s="4"/>
+      <c r="I2" s="3">
         <v>211</v>
       </c>
-      <c r="F2" s="5">
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="5">
         <v>165</v>
       </c>
-      <c r="G2" s="6">
+      <c r="M2" s="5"/>
+      <c r="N2" s="6">
         <v>123</v>
       </c>
-      <c r="H2" s="9">
+      <c r="O2" s="6"/>
+      <c r="P2" s="9">
         <v>249</v>
       </c>
-      <c r="I2" s="8">
+      <c r="Q2" s="9"/>
+      <c r="R2" s="8">
         <v>412</v>
       </c>
-      <c r="J2" s="10">
+      <c r="S2" s="8"/>
+      <c r="T2" s="10">
         <v>615</v>
       </c>
-      <c r="K2" s="7">
+      <c r="U2" s="10"/>
+      <c r="V2" s="7">
         <v>405</v>
       </c>
+      <c r="W2" s="7"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="2">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="2">
         <v>266</v>
       </c>
-      <c r="D3" s="4">
+      <c r="F3" s="2"/>
+      <c r="G3" s="4">
         <v>353</v>
       </c>
-      <c r="E3" s="3">
+      <c r="H3" s="4"/>
+      <c r="I3" s="3">
         <v>321</v>
       </c>
-      <c r="F3" s="5">
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="5">
         <v>256</v>
       </c>
-      <c r="G3" s="6">
+      <c r="M3" s="5"/>
+      <c r="N3" s="6">
         <v>225</v>
       </c>
-      <c r="H3" s="9">
+      <c r="O3" s="6"/>
+      <c r="P3" s="9">
         <v>271</v>
       </c>
-      <c r="I3" s="8">
+      <c r="Q3" s="9"/>
+      <c r="R3" s="8">
         <v>279</v>
       </c>
-      <c r="J3" s="10">
+      <c r="S3" s="8"/>
+      <c r="T3" s="10">
         <v>220</v>
       </c>
-      <c r="K3" s="7">
+      <c r="U3" s="10"/>
+      <c r="V3" s="7">
         <v>158</v>
       </c>
+      <c r="W3" s="7"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="2">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="2">
         <v>1</v>
       </c>
-      <c r="D4" s="4">
+      <c r="F4" s="2"/>
+      <c r="G4" s="4">
         <v>1950</v>
       </c>
-      <c r="E4" s="3">
+      <c r="H4" s="4"/>
+      <c r="I4" s="3">
         <v>816</v>
       </c>
-      <c r="F4" s="5">
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="5">
         <v>630</v>
       </c>
-      <c r="G4" s="6">
+      <c r="M4" s="5"/>
+      <c r="N4" s="6">
         <v>711</v>
       </c>
-      <c r="H4" s="9">
+      <c r="O4" s="6"/>
+      <c r="P4" s="9">
         <v>930</v>
       </c>
-      <c r="I4" s="8">
+      <c r="Q4" s="9"/>
+      <c r="R4" s="8">
         <v>1360</v>
       </c>
-      <c r="J4" s="10">
+      <c r="S4" s="8"/>
+      <c r="T4" s="10">
         <v>1</v>
       </c>
-      <c r="K4" s="7">
+      <c r="U4" s="10"/>
+      <c r="V4" s="7">
         <v>1233</v>
       </c>
+      <c r="W4" s="7"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="2">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="4">
+      <c r="F5" s="2"/>
+      <c r="G5" s="4">
         <v>1</v>
       </c>
-      <c r="E5" s="3">
+      <c r="H5" s="4"/>
+      <c r="I5" s="3">
         <v>1421</v>
       </c>
-      <c r="F5" s="5">
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="5">
         <v>1695</v>
       </c>
-      <c r="G5" s="6">
+      <c r="M5" s="5"/>
+      <c r="N5" s="6">
         <v>1299</v>
       </c>
-      <c r="H5" s="9">
+      <c r="O5" s="6"/>
+      <c r="P5" s="9">
         <v>1415</v>
       </c>
-      <c r="I5" s="8">
+      <c r="Q5" s="9"/>
+      <c r="R5" s="8">
         <v>1</v>
       </c>
-      <c r="J5" s="10">
+      <c r="S5" s="8"/>
+      <c r="T5" s="10">
         <v>1</v>
       </c>
-      <c r="K5" s="7">
+      <c r="U5" s="10"/>
+      <c r="V5" s="7">
         <v>1160</v>
       </c>
+      <c r="W5" s="7"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="2">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="2">
         <v>240</v>
       </c>
-      <c r="D6" s="4">
+      <c r="F6" s="2"/>
+      <c r="G6" s="4">
         <v>278</v>
       </c>
-      <c r="E6" s="3">
+      <c r="H6" s="4"/>
+      <c r="I6" s="3">
         <v>258</v>
       </c>
-      <c r="F6" s="5">
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="5">
         <v>259</v>
       </c>
-      <c r="G6" s="6">
+      <c r="M6" s="5"/>
+      <c r="N6" s="6">
         <v>250</v>
       </c>
-      <c r="H6" s="9">
+      <c r="O6" s="6"/>
+      <c r="P6" s="9">
         <v>280</v>
       </c>
-      <c r="I6" s="8">
+      <c r="Q6" s="9"/>
+      <c r="R6" s="8">
         <v>300</v>
       </c>
-      <c r="J6" s="10">
+      <c r="S6" s="8"/>
+      <c r="T6" s="10">
         <v>280</v>
       </c>
-      <c r="K6" s="7">
+      <c r="U6" s="10"/>
+      <c r="V6" s="7">
         <v>215</v>
       </c>
-      <c r="M6" t="s">
+      <c r="W6" s="7"/>
+      <c r="Z6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="2">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="2">
         <v>1056</v>
       </c>
-      <c r="D7" s="4">
+      <c r="F7" s="2"/>
+      <c r="G7" s="4">
         <v>1125</v>
       </c>
-      <c r="E7" s="3">
+      <c r="H7" s="4"/>
+      <c r="I7" s="3">
         <v>1030</v>
       </c>
-      <c r="F7" s="5">
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="5">
         <v>1017</v>
       </c>
-      <c r="G7" s="6">
+      <c r="M7" s="5"/>
+      <c r="N7" s="6">
         <v>983</v>
       </c>
-      <c r="H7" s="9">
+      <c r="O7" s="6"/>
+      <c r="P7" s="9">
         <v>1075</v>
       </c>
-      <c r="I7" s="8">
+      <c r="Q7" s="9"/>
+      <c r="R7" s="8">
         <v>1200</v>
       </c>
-      <c r="J7" s="10">
+      <c r="S7" s="8"/>
+      <c r="T7" s="10">
         <v>1040</v>
       </c>
-      <c r="K7" s="7">
+      <c r="U7" s="10"/>
+      <c r="V7" s="7">
         <v>593</v>
       </c>
+      <c r="W7" s="7"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="2">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2">
         <v>331</v>
       </c>
-      <c r="D8" s="4">
+      <c r="F8" s="2"/>
+      <c r="G8" s="4">
         <v>550</v>
       </c>
-      <c r="E8" s="3">
+      <c r="H8" s="4"/>
+      <c r="I8" s="3">
         <v>575</v>
       </c>
-      <c r="F8" s="5">
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="5">
         <v>532</v>
       </c>
-      <c r="G8" s="6">
+      <c r="M8" s="5"/>
+      <c r="N8" s="6">
         <v>510</v>
       </c>
-      <c r="H8" s="9">
+      <c r="O8" s="6"/>
+      <c r="P8" s="9">
         <v>608</v>
       </c>
-      <c r="I8" s="8">
+      <c r="Q8" s="9"/>
+      <c r="R8" s="8">
         <v>72</v>
       </c>
-      <c r="J8" s="10">
+      <c r="S8" s="8"/>
+      <c r="T8" s="10">
         <v>623</v>
       </c>
-      <c r="K8" s="7">
+      <c r="U8" s="10"/>
+      <c r="V8" s="7">
         <v>395</v>
       </c>
+      <c r="W8" s="7"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="2">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="2">
         <v>198</v>
       </c>
-      <c r="D9" s="4">
+      <c r="F9" s="2"/>
+      <c r="G9" s="4">
         <v>252</v>
       </c>
-      <c r="E9" s="3">
+      <c r="H9" s="4"/>
+      <c r="I9" s="3">
         <v>230</v>
       </c>
-      <c r="F9" s="5">
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="5">
         <v>147</v>
       </c>
-      <c r="G9" s="6">
+      <c r="M9" s="5"/>
+      <c r="N9" s="6">
         <v>227</v>
       </c>
-      <c r="H9" s="9">
+      <c r="O9" s="6"/>
+      <c r="P9" s="9">
         <v>253</v>
       </c>
-      <c r="I9" s="8">
+      <c r="Q9" s="9"/>
+      <c r="R9" s="8">
         <v>247</v>
       </c>
-      <c r="J9" s="10">
+      <c r="S9" s="8"/>
+      <c r="T9" s="10">
         <v>190</v>
       </c>
-      <c r="K9" s="7">
+      <c r="U9" s="10"/>
+      <c r="V9" s="7">
         <v>140</v>
       </c>
+      <c r="W9" s="7"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="2">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="2">
         <v>125</v>
       </c>
-      <c r="D10" s="4">
+      <c r="F10" s="2"/>
+      <c r="G10" s="4">
         <v>152</v>
       </c>
-      <c r="E10" s="3">
+      <c r="H10" s="4"/>
+      <c r="I10" s="3">
         <v>157</v>
       </c>
-      <c r="F10" s="5">
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="5">
         <v>137</v>
       </c>
-      <c r="G10" s="6">
+      <c r="M10" s="5"/>
+      <c r="N10" s="6">
         <v>141</v>
       </c>
-      <c r="H10" s="9">
+      <c r="O10" s="6"/>
+      <c r="P10" s="9">
         <v>262</v>
       </c>
-      <c r="I10" s="8">
+      <c r="Q10" s="9"/>
+      <c r="R10" s="8">
         <v>497</v>
       </c>
-      <c r="J10" s="10">
+      <c r="S10" s="8"/>
+      <c r="T10" s="10">
         <v>725</v>
       </c>
-      <c r="K10" s="7">
+      <c r="U10" s="10"/>
+      <c r="V10" s="7">
         <v>460</v>
       </c>
+      <c r="W10" s="7"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="2">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="2">
         <v>163</v>
       </c>
-      <c r="D11" s="4">
+      <c r="F11" s="2"/>
+      <c r="G11" s="4">
         <v>252</v>
       </c>
-      <c r="E11" s="3">
+      <c r="H11" s="4"/>
+      <c r="I11" s="3">
         <v>165</v>
       </c>
-      <c r="F11" s="5">
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="5">
         <v>137</v>
       </c>
-      <c r="G11" s="6">
+      <c r="M11" s="5"/>
+      <c r="N11" s="6">
         <v>133</v>
       </c>
-      <c r="H11" s="9">
+      <c r="O11" s="6"/>
+      <c r="P11" s="9">
         <v>181</v>
       </c>
-      <c r="I11" s="8">
+      <c r="Q11" s="9"/>
+      <c r="R11" s="8">
         <v>189</v>
       </c>
-      <c r="J11" s="10">
+      <c r="S11" s="8"/>
+      <c r="T11" s="10">
         <v>369</v>
       </c>
-      <c r="K11" s="7">
+      <c r="U11" s="10"/>
+      <c r="V11" s="7">
         <v>256</v>
       </c>
+      <c r="W11" s="7"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="1"/>
-      <c r="C12" s="2">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2">
         <v>260</v>
       </c>
-      <c r="D12" s="4">
+      <c r="F12" s="2"/>
+      <c r="G12" s="4">
         <v>145</v>
       </c>
-      <c r="E12" s="3">
+      <c r="H12" s="4"/>
+      <c r="I12" s="3">
         <v>138</v>
       </c>
-      <c r="F12" s="5">
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="5">
         <v>130</v>
       </c>
-      <c r="G12" s="6">
+      <c r="M12" s="5"/>
+      <c r="N12" s="6">
         <v>128</v>
       </c>
-      <c r="H12" s="9">
+      <c r="O12" s="6"/>
+      <c r="P12" s="9">
         <v>213</v>
       </c>
-      <c r="I12" s="8">
+      <c r="Q12" s="9"/>
+      <c r="R12" s="8">
         <v>209</v>
       </c>
-      <c r="J12" s="10">
+      <c r="S12" s="8"/>
+      <c r="T12" s="10">
         <v>524</v>
       </c>
-      <c r="K12" s="7">
+      <c r="U12" s="10"/>
+      <c r="V12" s="7">
         <v>354</v>
       </c>
+      <c r="W12" s="7"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="1"/>
-      <c r="C13" s="2">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="2">
         <v>355</v>
       </c>
-      <c r="D13" s="4">
+      <c r="F13" s="2"/>
+      <c r="G13" s="4">
         <v>690</v>
       </c>
-      <c r="E13" s="3">
+      <c r="H13" s="4"/>
+      <c r="I13" s="3">
         <v>463</v>
       </c>
-      <c r="F13" s="5">
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="5">
         <v>385</v>
       </c>
-      <c r="G13" s="6">
+      <c r="M13" s="5"/>
+      <c r="N13" s="6">
         <v>367</v>
       </c>
-      <c r="H13" s="9">
+      <c r="O13" s="6"/>
+      <c r="P13" s="9">
         <v>510</v>
       </c>
-      <c r="I13" s="8">
+      <c r="Q13" s="9"/>
+      <c r="R13" s="8">
         <v>634</v>
       </c>
-      <c r="J13" s="10">
+      <c r="S13" s="8"/>
+      <c r="T13" s="10">
         <v>900</v>
       </c>
-      <c r="K13" s="7">
+      <c r="U13" s="10"/>
+      <c r="V13" s="7">
         <v>577</v>
       </c>
+      <c r="W13" s="7"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="2">
+      <c r="E14" s="2">
         <v>387</v>
       </c>
-      <c r="D14" s="4">
+      <c r="F14" s="2"/>
+      <c r="G14" s="4">
         <v>1242</v>
       </c>
-      <c r="E14" s="3">
+      <c r="H14" s="4"/>
+      <c r="I14" s="3">
         <v>1222</v>
       </c>
-      <c r="F14" s="5">
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="5">
         <v>1104</v>
       </c>
-      <c r="G14" s="6">
+      <c r="M14" s="5"/>
+      <c r="N14" s="6">
         <v>1084</v>
       </c>
-      <c r="H14" s="9">
+      <c r="O14" s="6"/>
+      <c r="P14" s="9">
         <v>1199</v>
       </c>
-      <c r="I14" s="8">
+      <c r="Q14" s="9"/>
+      <c r="R14" s="8">
         <v>1271</v>
       </c>
-      <c r="J14" s="10">
+      <c r="S14" s="8"/>
+      <c r="T14" s="10">
         <v>1050</v>
       </c>
-      <c r="K14" s="7">
+      <c r="U14" s="10"/>
+      <c r="V14" s="7">
         <v>644</v>
       </c>
+      <c r="W14" s="7"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="2">
+      <c r="E15" s="2">
         <v>211</v>
       </c>
-      <c r="D15" s="4">
+      <c r="F15" s="2"/>
+      <c r="G15" s="4">
         <v>234</v>
       </c>
-      <c r="E15" s="3">
+      <c r="H15" s="4"/>
+      <c r="I15" s="3">
         <v>374</v>
       </c>
-      <c r="F15" s="5">
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="5">
         <v>520</v>
       </c>
-      <c r="G15" s="6">
+      <c r="M15" s="5"/>
+      <c r="N15" s="6">
         <v>602</v>
       </c>
-      <c r="H15" s="9">
+      <c r="O15" s="6"/>
+      <c r="P15" s="9">
         <v>719</v>
       </c>
-      <c r="I15" s="8">
+      <c r="Q15" s="9"/>
+      <c r="R15" s="8">
         <v>804</v>
       </c>
-      <c r="J15" s="10">
+      <c r="S15" s="8"/>
+      <c r="T15" s="10">
         <v>765</v>
       </c>
-      <c r="K15" s="7">
+      <c r="U15" s="10"/>
+      <c r="V15" s="7">
         <v>465</v>
       </c>
+      <c r="W15" s="7"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="2">
+      <c r="E16" s="2">
         <v>393</v>
       </c>
-      <c r="D16" s="4">
+      <c r="F16" s="2"/>
+      <c r="G16" s="4">
         <v>1221</v>
       </c>
-      <c r="E16" s="3">
+      <c r="H16" s="4"/>
+      <c r="I16" s="3">
         <v>1219</v>
       </c>
-      <c r="F16" s="5">
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="5">
         <v>1134</v>
       </c>
-      <c r="G16" s="6">
+      <c r="M16" s="5"/>
+      <c r="N16" s="6">
         <v>1119</v>
       </c>
-      <c r="H16" s="9">
+      <c r="O16" s="6"/>
+      <c r="P16" s="9">
         <v>1250</v>
       </c>
-      <c r="I16" s="8">
+      <c r="Q16" s="9"/>
+      <c r="R16" s="8">
         <v>1353</v>
       </c>
-      <c r="J16" s="10">
+      <c r="S16" s="8"/>
+      <c r="T16" s="10">
         <v>1195</v>
       </c>
-      <c r="K16" s="7">
+      <c r="U16" s="10"/>
+      <c r="V16" s="7">
         <v>692</v>
       </c>
+      <c r="W16" s="7"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C18" s="1" t="s">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="E18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="F18" s="1"/>
+      <c r="G18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="H18" s="1"/>
+      <c r="I18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="M18" s="1"/>
+      <c r="N18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="O18" s="1"/>
+      <c r="P18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="S18" s="1"/>
+      <c r="T18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="U18" s="1"/>
+      <c r="V18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="W18" s="1"/>
+      <c r="X18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N18" s="1" t="s">
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O18" t="s">
+      <c r="AC18" s="1"/>
+      <c r="AD18" t="s">
         <v>12</v>
       </c>
-      <c r="P18" t="s">
+      <c r="AF18" t="s">
         <v>13</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="AH18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="11">
         <v>470</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="11">
+        <v>470</v>
+      </c>
+      <c r="D19" s="2">
         <v>151</v>
       </c>
-      <c r="D19" s="2">
+      <c r="E19" s="2">
+        <f>(D19/2000)*100</f>
+        <v>7.55</v>
+      </c>
+      <c r="F19" s="2">
         <v>266</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
       <c r="G19" s="2">
+        <f>(F19/2000)*100</f>
+        <v>13.3</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2">
         <v>240</v>
       </c>
-      <c r="H19" s="2">
+      <c r="N19" s="2">
+        <f>(M19/2000)*100</f>
+        <v>12</v>
+      </c>
+      <c r="O19" s="2">
         <v>1056</v>
       </c>
-      <c r="I19" s="2">
+      <c r="P19" s="2">
+        <f>(O19/2000)*100</f>
+        <v>52.800000000000004</v>
+      </c>
+      <c r="Q19" s="2">
         <v>331</v>
       </c>
-      <c r="J19" s="2">
+      <c r="R19" s="2">
+        <f>(Q19/2000)*100</f>
+        <v>16.55</v>
+      </c>
+      <c r="S19" s="2">
         <v>198</v>
       </c>
-      <c r="K19" s="2">
+      <c r="T19" s="2">
+        <f>(S19/2000)*100</f>
+        <v>9.9</v>
+      </c>
+      <c r="U19" s="2">
         <v>125</v>
       </c>
-      <c r="L19" s="2">
+      <c r="V19" s="2">
+        <f>(U19/2000)*100</f>
+        <v>6.25</v>
+      </c>
+      <c r="W19" s="2">
         <v>163</v>
       </c>
-      <c r="M19" s="2">
+      <c r="X19" s="2">
+        <f>(W19/2000)*100</f>
+        <v>8.15</v>
+      </c>
+      <c r="Y19" s="2">
         <v>260</v>
       </c>
-      <c r="N19" s="2">
+      <c r="Z19" s="2">
+        <f>(Y19/2000)*100</f>
+        <v>13</v>
+      </c>
+      <c r="AA19" s="2">
         <v>355</v>
       </c>
-      <c r="O19" s="2">
+      <c r="AB19" s="2">
+        <f>(AA19/2000)*100</f>
+        <v>17.75</v>
+      </c>
+      <c r="AC19" s="2">
         <v>387</v>
       </c>
-      <c r="P19" s="2">
+      <c r="AD19" s="2">
+        <f>(AC19/2000)*100</f>
+        <v>19.350000000000001</v>
+      </c>
+      <c r="AE19" s="2">
         <v>211</v>
       </c>
-      <c r="Q19" s="2">
+      <c r="AF19" s="2">
+        <f>(AE19/2000)*100</f>
+        <v>10.549999999999999</v>
+      </c>
+      <c r="AG19" s="2">
         <v>393</v>
       </c>
+      <c r="AH19" s="2">
+        <f>(AG19/2000)*100</f>
+        <v>19.650000000000002</v>
+      </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
       <c r="B20">
         <v>555</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20">
+        <v>555</v>
+      </c>
+      <c r="D20" s="4">
         <v>280</v>
       </c>
-      <c r="D20" s="4">
+      <c r="E20" s="2">
+        <f t="shared" ref="E20:E27" si="0">(D20/2000)*100</f>
+        <v>14.000000000000002</v>
+      </c>
+      <c r="F20" s="4">
         <v>353</v>
       </c>
-      <c r="E20" s="4">
+      <c r="G20" s="2">
+        <f t="shared" ref="G20:G27" si="1">(F20/2000)*100</f>
+        <v>17.649999999999999</v>
+      </c>
+      <c r="H20" s="4">
         <v>1950</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4">
+      <c r="I20" s="4">
+        <f>(H20/2000)*100</f>
+        <v>97.5</v>
+      </c>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4">
         <v>278</v>
       </c>
-      <c r="H20" s="4">
+      <c r="N20" s="2">
+        <f t="shared" ref="N20:N27" si="2">(M20/2000)*100</f>
+        <v>13.900000000000002</v>
+      </c>
+      <c r="O20" s="4">
         <v>1125</v>
       </c>
-      <c r="I20" s="4">
+      <c r="P20" s="2">
+        <f t="shared" ref="P20:P27" si="3">(O20/2000)*100</f>
+        <v>56.25</v>
+      </c>
+      <c r="Q20" s="4">
         <v>550</v>
       </c>
-      <c r="J20" s="4">
+      <c r="R20" s="2">
+        <f t="shared" ref="R20:R27" si="4">(Q20/2000)*100</f>
+        <v>27.500000000000004</v>
+      </c>
+      <c r="S20" s="4">
         <v>252</v>
       </c>
-      <c r="K20" s="4">
+      <c r="T20" s="2">
+        <f t="shared" ref="T20:T27" si="5">(S20/2000)*100</f>
+        <v>12.6</v>
+      </c>
+      <c r="U20" s="4">
         <v>152</v>
       </c>
-      <c r="L20" s="4">
+      <c r="V20" s="2">
+        <f t="shared" ref="V20:V27" si="6">(U20/2000)*100</f>
+        <v>7.6</v>
+      </c>
+      <c r="W20" s="4">
         <v>252</v>
       </c>
-      <c r="M20" s="4">
+      <c r="X20" s="2">
+        <f t="shared" ref="X20:X27" si="7">(W20/2000)*100</f>
+        <v>12.6</v>
+      </c>
+      <c r="Y20" s="4">
         <v>145</v>
       </c>
-      <c r="N20" s="4">
+      <c r="Z20" s="2">
+        <f t="shared" ref="Z20:Z27" si="8">(Y20/2000)*100</f>
+        <v>7.2499999999999991</v>
+      </c>
+      <c r="AA20" s="4">
         <v>690</v>
       </c>
-      <c r="O20" s="4">
+      <c r="AB20" s="2">
+        <f t="shared" ref="AB20:AB27" si="9">(AA20/2000)*100</f>
+        <v>34.5</v>
+      </c>
+      <c r="AC20" s="4">
         <v>1242</v>
       </c>
-      <c r="P20" s="4">
+      <c r="AD20" s="2">
+        <f t="shared" ref="AD20:AD27" si="10">(AC20/2000)*100</f>
+        <v>62.1</v>
+      </c>
+      <c r="AE20" s="4">
         <v>234</v>
       </c>
-      <c r="Q20" s="4">
+      <c r="AF20" s="2">
+        <f t="shared" ref="AF20:AF27" si="11">(AE20/2000)*100</f>
+        <v>11.700000000000001</v>
+      </c>
+      <c r="AG20" s="4">
         <v>1221</v>
       </c>
+      <c r="AH20" s="2">
+        <f t="shared" ref="AH20:AH27" si="12">(AG20/2000)*100</f>
+        <v>61.050000000000004</v>
+      </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
       <c r="B21">
         <v>585</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21">
+        <v>585</v>
+      </c>
+      <c r="D21" s="3">
         <v>211</v>
       </c>
-      <c r="D21" s="3">
+      <c r="E21" s="2">
+        <f t="shared" si="0"/>
+        <v>10.549999999999999</v>
+      </c>
+      <c r="F21" s="3">
         <v>321</v>
       </c>
-      <c r="E21" s="3">
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>16.05</v>
+      </c>
+      <c r="H21" s="3">
         <v>816</v>
       </c>
-      <c r="F21" s="3">
+      <c r="I21" s="4">
+        <f t="shared" ref="I21:I27" si="13">(H21/2000)*100</f>
+        <v>40.799999999999997</v>
+      </c>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3">
         <v>1421</v>
       </c>
-      <c r="G21" s="3">
+      <c r="L21" s="3">
+        <f>(K21/2000)*100</f>
+        <v>71.05</v>
+      </c>
+      <c r="M21" s="3">
         <v>258</v>
       </c>
-      <c r="H21" s="3">
+      <c r="N21" s="2">
+        <f t="shared" si="2"/>
+        <v>12.9</v>
+      </c>
+      <c r="O21" s="3">
         <v>1030</v>
       </c>
-      <c r="I21" s="3">
+      <c r="P21" s="2">
+        <f t="shared" si="3"/>
+        <v>51.5</v>
+      </c>
+      <c r="Q21" s="3">
         <v>575</v>
       </c>
-      <c r="J21" s="3">
+      <c r="R21" s="2">
+        <f t="shared" si="4"/>
+        <v>28.749999999999996</v>
+      </c>
+      <c r="S21" s="3">
         <v>230</v>
       </c>
-      <c r="K21" s="3">
+      <c r="T21" s="2">
+        <f t="shared" si="5"/>
+        <v>11.5</v>
+      </c>
+      <c r="U21" s="3">
         <v>157</v>
       </c>
-      <c r="L21" s="3">
+      <c r="V21" s="2">
+        <f t="shared" si="6"/>
+        <v>7.85</v>
+      </c>
+      <c r="W21" s="3">
         <v>165</v>
       </c>
-      <c r="M21" s="3">
+      <c r="X21" s="2">
+        <f t="shared" si="7"/>
+        <v>8.25</v>
+      </c>
+      <c r="Y21" s="3">
         <v>138</v>
       </c>
-      <c r="N21" s="3">
+      <c r="Z21" s="2">
+        <f t="shared" si="8"/>
+        <v>6.9</v>
+      </c>
+      <c r="AA21" s="3">
         <v>463</v>
       </c>
-      <c r="O21" s="3">
+      <c r="AB21" s="2">
+        <f t="shared" si="9"/>
+        <v>23.150000000000002</v>
+      </c>
+      <c r="AC21" s="3">
         <v>1222</v>
       </c>
-      <c r="P21" s="3">
+      <c r="AD21" s="2">
+        <f t="shared" si="10"/>
+        <v>61.1</v>
+      </c>
+      <c r="AE21" s="3">
         <v>374</v>
       </c>
-      <c r="Q21" s="3">
+      <c r="AF21" s="2">
+        <f t="shared" si="11"/>
+        <v>18.7</v>
+      </c>
+      <c r="AG21" s="3">
         <v>1219</v>
       </c>
+      <c r="AH21" s="2">
+        <f t="shared" si="12"/>
+        <v>60.95</v>
+      </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
       <c r="B22">
         <v>605</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22">
+        <v>605</v>
+      </c>
+      <c r="D22" s="5">
         <v>165</v>
       </c>
-      <c r="D22" s="5">
+      <c r="E22" s="2">
+        <f t="shared" si="0"/>
+        <v>8.25</v>
+      </c>
+      <c r="F22" s="5">
         <v>256</v>
       </c>
-      <c r="E22" s="5">
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>12.8</v>
+      </c>
+      <c r="H22" s="5">
         <v>630</v>
       </c>
-      <c r="F22" s="5">
+      <c r="I22" s="4">
+        <f t="shared" si="13"/>
+        <v>31.5</v>
+      </c>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5">
         <v>1695</v>
       </c>
-      <c r="G22" s="5">
+      <c r="L22" s="3">
+        <f t="shared" ref="L22:L27" si="14">(K22/2000)*100</f>
+        <v>84.75</v>
+      </c>
+      <c r="M22" s="5">
         <v>259</v>
       </c>
-      <c r="H22" s="5">
+      <c r="N22" s="2">
+        <f t="shared" si="2"/>
+        <v>12.950000000000001</v>
+      </c>
+      <c r="O22" s="5">
         <v>1017</v>
       </c>
-      <c r="I22" s="5">
+      <c r="P22" s="2">
+        <f t="shared" si="3"/>
+        <v>50.849999999999994</v>
+      </c>
+      <c r="Q22" s="5">
         <v>532</v>
       </c>
-      <c r="J22" s="5">
+      <c r="R22" s="2">
+        <f t="shared" si="4"/>
+        <v>26.6</v>
+      </c>
+      <c r="S22" s="5">
         <v>147</v>
       </c>
-      <c r="K22" s="5">
+      <c r="T22" s="2">
+        <f t="shared" si="5"/>
+        <v>7.35</v>
+      </c>
+      <c r="U22" s="5">
         <v>137</v>
       </c>
-      <c r="L22" s="5">
+      <c r="V22" s="2">
+        <f t="shared" si="6"/>
+        <v>6.8500000000000005</v>
+      </c>
+      <c r="W22" s="5">
         <v>137</v>
       </c>
-      <c r="M22" s="5">
+      <c r="X22" s="2">
+        <f t="shared" si="7"/>
+        <v>6.8500000000000005</v>
+      </c>
+      <c r="Y22" s="5">
         <v>130</v>
       </c>
-      <c r="N22" s="5">
+      <c r="Z22" s="2">
+        <f t="shared" si="8"/>
+        <v>6.5</v>
+      </c>
+      <c r="AA22" s="5">
         <v>385</v>
       </c>
-      <c r="O22" s="5">
+      <c r="AB22" s="2">
+        <f t="shared" si="9"/>
+        <v>19.25</v>
+      </c>
+      <c r="AC22" s="5">
         <v>1104</v>
       </c>
-      <c r="P22" s="5">
+      <c r="AD22" s="2">
+        <f t="shared" si="10"/>
+        <v>55.2</v>
+      </c>
+      <c r="AE22" s="5">
         <v>520</v>
       </c>
-      <c r="Q22" s="5">
+      <c r="AF22" s="2">
+        <f t="shared" si="11"/>
+        <v>26</v>
+      </c>
+      <c r="AG22" s="5">
         <v>1134</v>
       </c>
-      <c r="S22" t="s">
+      <c r="AH22" s="2">
+        <f t="shared" si="12"/>
+        <v>56.699999999999996</v>
+      </c>
+      <c r="AJ22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
       <c r="B23">
         <v>635</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23">
+        <v>635</v>
+      </c>
+      <c r="D23" s="6">
         <v>123</v>
       </c>
-      <c r="D23" s="6">
+      <c r="E23" s="2">
+        <f t="shared" si="0"/>
+        <v>6.15</v>
+      </c>
+      <c r="F23" s="6">
         <v>225</v>
       </c>
-      <c r="E23" s="6">
+      <c r="G23" s="2">
+        <f t="shared" si="1"/>
+        <v>11.25</v>
+      </c>
+      <c r="H23" s="6">
         <v>711</v>
       </c>
-      <c r="F23" s="6">
+      <c r="I23" s="4">
+        <f t="shared" si="13"/>
+        <v>35.549999999999997</v>
+      </c>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6">
         <v>1299</v>
       </c>
-      <c r="G23" s="6">
+      <c r="L23" s="3">
+        <f t="shared" si="14"/>
+        <v>64.95</v>
+      </c>
+      <c r="M23" s="6">
         <v>250</v>
       </c>
-      <c r="H23" s="6">
+      <c r="N23" s="2">
+        <f t="shared" si="2"/>
+        <v>12.5</v>
+      </c>
+      <c r="O23" s="6">
         <v>983</v>
       </c>
-      <c r="I23" s="6">
+      <c r="P23" s="2">
+        <f t="shared" si="3"/>
+        <v>49.15</v>
+      </c>
+      <c r="Q23" s="6">
         <v>510</v>
       </c>
-      <c r="J23" s="6">
+      <c r="R23" s="2">
+        <f t="shared" si="4"/>
+        <v>25.5</v>
+      </c>
+      <c r="S23" s="6">
         <v>227</v>
       </c>
-      <c r="K23" s="6">
+      <c r="T23" s="2">
+        <f t="shared" si="5"/>
+        <v>11.35</v>
+      </c>
+      <c r="U23" s="6">
         <v>141</v>
       </c>
-      <c r="L23" s="6">
+      <c r="V23" s="2">
+        <f t="shared" si="6"/>
+        <v>7.0499999999999989</v>
+      </c>
+      <c r="W23" s="6">
         <v>133</v>
       </c>
-      <c r="M23" s="6">
+      <c r="X23" s="2">
+        <f t="shared" si="7"/>
+        <v>6.65</v>
+      </c>
+      <c r="Y23" s="6">
         <v>128</v>
       </c>
-      <c r="N23" s="6">
+      <c r="Z23" s="2">
+        <f t="shared" si="8"/>
+        <v>6.4</v>
+      </c>
+      <c r="AA23" s="6">
         <v>367</v>
       </c>
-      <c r="O23" s="6">
+      <c r="AB23" s="2">
+        <f t="shared" si="9"/>
+        <v>18.350000000000001</v>
+      </c>
+      <c r="AC23" s="6">
         <v>1084</v>
       </c>
-      <c r="P23" s="6">
+      <c r="AD23" s="2">
+        <f t="shared" si="10"/>
+        <v>54.2</v>
+      </c>
+      <c r="AE23" s="6">
         <v>602</v>
       </c>
-      <c r="Q23" s="6">
+      <c r="AF23" s="2">
+        <f t="shared" si="11"/>
+        <v>30.099999999999998</v>
+      </c>
+      <c r="AG23" s="6">
         <v>1119</v>
       </c>
+      <c r="AH23" s="2">
+        <f t="shared" si="12"/>
+        <v>55.95</v>
+      </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
       <c r="B24">
         <v>660</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24">
+        <v>660</v>
+      </c>
+      <c r="D24" s="9">
         <v>249</v>
       </c>
-      <c r="D24" s="9">
+      <c r="E24" s="2">
+        <f t="shared" si="0"/>
+        <v>12.45</v>
+      </c>
+      <c r="F24" s="9">
         <v>271</v>
       </c>
-      <c r="E24" s="9">
+      <c r="G24" s="2">
+        <f t="shared" si="1"/>
+        <v>13.55</v>
+      </c>
+      <c r="H24" s="9">
         <v>930</v>
       </c>
-      <c r="F24" s="9">
+      <c r="I24" s="4">
+        <f t="shared" si="13"/>
+        <v>46.5</v>
+      </c>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9">
         <v>1415</v>
       </c>
-      <c r="G24" s="9">
+      <c r="L24" s="3">
+        <f t="shared" si="14"/>
+        <v>70.75</v>
+      </c>
+      <c r="M24" s="9">
         <v>280</v>
       </c>
-      <c r="H24" s="9">
+      <c r="N24" s="2">
+        <f t="shared" si="2"/>
+        <v>14.000000000000002</v>
+      </c>
+      <c r="O24" s="9">
         <v>1075</v>
       </c>
-      <c r="I24" s="9">
+      <c r="P24" s="2">
+        <f t="shared" si="3"/>
+        <v>53.75</v>
+      </c>
+      <c r="Q24" s="9">
         <v>608</v>
       </c>
-      <c r="J24" s="9">
+      <c r="R24" s="2">
+        <f t="shared" si="4"/>
+        <v>30.4</v>
+      </c>
+      <c r="S24" s="9">
         <v>253</v>
       </c>
-      <c r="K24" s="9">
+      <c r="T24" s="2">
+        <f t="shared" si="5"/>
+        <v>12.65</v>
+      </c>
+      <c r="U24" s="9">
         <v>262</v>
       </c>
-      <c r="L24" s="9">
+      <c r="V24" s="2">
+        <f t="shared" si="6"/>
+        <v>13.100000000000001</v>
+      </c>
+      <c r="W24" s="9">
         <v>181</v>
       </c>
-      <c r="M24" s="9">
+      <c r="X24" s="2">
+        <f t="shared" si="7"/>
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="Y24" s="9">
         <v>213</v>
       </c>
-      <c r="N24" s="9">
+      <c r="Z24" s="2">
+        <f t="shared" si="8"/>
+        <v>10.65</v>
+      </c>
+      <c r="AA24" s="9">
         <v>510</v>
       </c>
-      <c r="O24" s="9">
+      <c r="AB24" s="2">
+        <f t="shared" si="9"/>
+        <v>25.5</v>
+      </c>
+      <c r="AC24" s="9">
         <v>1199</v>
       </c>
-      <c r="P24" s="9">
+      <c r="AD24" s="2">
+        <f t="shared" si="10"/>
+        <v>59.95</v>
+      </c>
+      <c r="AE24" s="9">
         <v>719</v>
       </c>
-      <c r="Q24" s="9">
+      <c r="AF24" s="2">
+        <f t="shared" si="11"/>
+        <v>35.949999999999996</v>
+      </c>
+      <c r="AG24" s="9">
         <v>1250</v>
       </c>
+      <c r="AH24" s="2">
+        <f t="shared" si="12"/>
+        <v>62.5</v>
+      </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
       <c r="B25">
         <v>695</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25">
+        <v>695</v>
+      </c>
+      <c r="D25" s="8">
         <v>412</v>
       </c>
-      <c r="D25" s="8">
+      <c r="E25" s="2">
+        <f t="shared" si="0"/>
+        <v>20.599999999999998</v>
+      </c>
+      <c r="F25" s="8">
         <v>279</v>
       </c>
-      <c r="E25" s="8">
+      <c r="G25" s="2">
+        <f t="shared" si="1"/>
+        <v>13.950000000000001</v>
+      </c>
+      <c r="H25" s="8">
         <v>1360</v>
       </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8">
+      <c r="I25" s="4">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="8">
         <v>300</v>
       </c>
-      <c r="H25" s="8">
+      <c r="N25" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="O25" s="8">
         <v>1200</v>
       </c>
-      <c r="I25" s="8">
+      <c r="P25" s="2">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="Q25" s="8">
         <v>72</v>
       </c>
-      <c r="J25" s="8">
+      <c r="R25" s="2">
+        <f t="shared" si="4"/>
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="S25" s="8">
         <v>247</v>
       </c>
-      <c r="K25" s="8">
+      <c r="T25" s="2">
+        <f t="shared" si="5"/>
+        <v>12.35</v>
+      </c>
+      <c r="U25" s="8">
         <v>497</v>
       </c>
-      <c r="L25" s="8">
+      <c r="V25" s="2">
+        <f t="shared" si="6"/>
+        <v>24.85</v>
+      </c>
+      <c r="W25" s="8">
         <v>189</v>
       </c>
-      <c r="M25" s="8">
+      <c r="X25" s="2">
+        <f t="shared" si="7"/>
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="Y25" s="8">
         <v>209</v>
       </c>
-      <c r="N25" s="8">
+      <c r="Z25" s="2">
+        <f t="shared" si="8"/>
+        <v>10.45</v>
+      </c>
+      <c r="AA25" s="8">
         <v>634</v>
       </c>
-      <c r="O25" s="8">
+      <c r="AB25" s="2">
+        <f t="shared" si="9"/>
+        <v>31.7</v>
+      </c>
+      <c r="AC25" s="8">
         <v>1271</v>
       </c>
-      <c r="P25" s="8">
+      <c r="AD25" s="2">
+        <f t="shared" si="10"/>
+        <v>63.55</v>
+      </c>
+      <c r="AE25" s="8">
         <v>804</v>
       </c>
-      <c r="Q25" s="8">
+      <c r="AF25" s="2">
+        <f t="shared" si="11"/>
+        <v>40.200000000000003</v>
+      </c>
+      <c r="AG25" s="8">
         <v>1353</v>
       </c>
+      <c r="AH25" s="2">
+        <f t="shared" si="12"/>
+        <v>67.650000000000006</v>
+      </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
       <c r="B26">
         <v>880</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26">
+        <v>880</v>
+      </c>
+      <c r="D26" s="10">
         <v>615</v>
       </c>
-      <c r="D26" s="10">
+      <c r="E26" s="2">
+        <f t="shared" si="0"/>
+        <v>30.75</v>
+      </c>
+      <c r="F26" s="10">
         <v>220</v>
       </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10">
+      <c r="G26" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="H26" s="10"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="10">
         <v>280</v>
       </c>
-      <c r="H26" s="10">
+      <c r="N26" s="2">
+        <f t="shared" si="2"/>
+        <v>14.000000000000002</v>
+      </c>
+      <c r="O26" s="10">
         <v>1040</v>
       </c>
-      <c r="I26" s="10">
+      <c r="P26" s="2">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="Q26" s="10">
         <v>623</v>
       </c>
-      <c r="J26" s="10">
+      <c r="R26" s="2">
+        <f t="shared" si="4"/>
+        <v>31.15</v>
+      </c>
+      <c r="S26" s="10">
         <v>190</v>
       </c>
-      <c r="K26" s="10">
+      <c r="T26" s="2">
+        <f t="shared" si="5"/>
+        <v>9.5</v>
+      </c>
+      <c r="U26" s="10">
         <v>725</v>
       </c>
-      <c r="L26" s="10">
+      <c r="V26" s="2">
+        <f t="shared" si="6"/>
+        <v>36.25</v>
+      </c>
+      <c r="W26" s="10">
         <v>369</v>
       </c>
-      <c r="M26" s="10">
+      <c r="X26" s="2">
+        <f t="shared" si="7"/>
+        <v>18.45</v>
+      </c>
+      <c r="Y26" s="10">
         <v>524</v>
       </c>
-      <c r="N26" s="10">
+      <c r="Z26" s="2">
+        <f t="shared" si="8"/>
+        <v>26.200000000000003</v>
+      </c>
+      <c r="AA26" s="10">
         <v>900</v>
       </c>
-      <c r="O26" s="10">
+      <c r="AB26" s="2">
+        <f t="shared" si="9"/>
+        <v>45</v>
+      </c>
+      <c r="AC26" s="10">
         <v>1050</v>
       </c>
-      <c r="P26" s="10">
+      <c r="AD26" s="2">
+        <f t="shared" si="10"/>
+        <v>52.5</v>
+      </c>
+      <c r="AE26" s="10">
         <v>765</v>
       </c>
-      <c r="Q26" s="10">
+      <c r="AF26" s="2">
+        <f t="shared" si="11"/>
+        <v>38.25</v>
+      </c>
+      <c r="AG26" s="10">
         <v>1195</v>
       </c>
+      <c r="AH26" s="2">
+        <f t="shared" si="12"/>
+        <v>59.75</v>
+      </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
       <c r="B27">
         <v>940</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27">
+        <v>940</v>
+      </c>
+      <c r="D27" s="7">
         <v>405</v>
       </c>
-      <c r="D27" s="7">
+      <c r="E27" s="2">
+        <f t="shared" si="0"/>
+        <v>20.25</v>
+      </c>
+      <c r="F27" s="7">
         <v>158</v>
       </c>
-      <c r="E27" s="7">
+      <c r="G27" s="2">
+        <f t="shared" si="1"/>
+        <v>7.9</v>
+      </c>
+      <c r="H27" s="7">
         <v>1233</v>
       </c>
-      <c r="F27" s="7">
+      <c r="I27" s="4">
+        <f t="shared" si="13"/>
+        <v>61.650000000000006</v>
+      </c>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7">
         <v>1160</v>
       </c>
-      <c r="G27" s="7">
+      <c r="L27" s="3">
+        <f t="shared" si="14"/>
+        <v>57.999999999999993</v>
+      </c>
+      <c r="M27" s="7">
         <v>215</v>
       </c>
-      <c r="H27" s="7">
+      <c r="N27" s="2">
+        <f t="shared" si="2"/>
+        <v>10.75</v>
+      </c>
+      <c r="O27" s="7">
         <v>593</v>
       </c>
-      <c r="I27" s="7">
+      <c r="P27" s="2">
+        <f t="shared" si="3"/>
+        <v>29.65</v>
+      </c>
+      <c r="Q27" s="7">
         <v>395</v>
       </c>
-      <c r="J27" s="7">
+      <c r="R27" s="2">
+        <f t="shared" si="4"/>
+        <v>19.75</v>
+      </c>
+      <c r="S27" s="7">
         <v>140</v>
       </c>
-      <c r="K27" s="7">
+      <c r="T27" s="2">
+        <f t="shared" si="5"/>
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="U27" s="7">
         <v>460</v>
       </c>
-      <c r="L27" s="7">
+      <c r="V27" s="2">
+        <f t="shared" si="6"/>
+        <v>23</v>
+      </c>
+      <c r="W27" s="7">
         <v>256</v>
       </c>
-      <c r="M27" s="7">
+      <c r="X27" s="2">
+        <f t="shared" si="7"/>
+        <v>12.8</v>
+      </c>
+      <c r="Y27" s="7">
         <v>354</v>
       </c>
-      <c r="N27" s="7">
+      <c r="Z27" s="2">
+        <f t="shared" si="8"/>
+        <v>17.7</v>
+      </c>
+      <c r="AA27" s="7">
         <v>577</v>
       </c>
-      <c r="O27" s="7">
+      <c r="AB27" s="2">
+        <f t="shared" si="9"/>
+        <v>28.849999999999998</v>
+      </c>
+      <c r="AC27" s="7">
         <v>644</v>
       </c>
-      <c r="P27" s="7">
+      <c r="AD27" s="2">
+        <f t="shared" si="10"/>
+        <v>32.200000000000003</v>
+      </c>
+      <c r="AE27" s="7">
         <v>465</v>
       </c>
-      <c r="Q27" s="7">
+      <c r="AF27" s="2">
+        <f t="shared" si="11"/>
+        <v>23.25</v>
+      </c>
+      <c r="AG27" s="7">
         <v>692</v>
+      </c>
+      <c r="AH27" s="2">
+        <f t="shared" si="12"/>
+        <v>34.599999999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
attempt to calibrate graphs
</commit_message>
<xml_diff>
--- a/Spectra.graphs.xlsx
+++ b/Spectra.graphs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29070" windowHeight="15870"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14430" windowHeight="15630" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="27">
   <si>
     <t>Leaf:</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Reference</t>
   </si>
 </sst>
 </file>
@@ -1860,11 +1863,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="296490040"/>
-        <c:axId val="296522408"/>
+        <c:axId val="297827064"/>
+        <c:axId val="297862176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="296490040"/>
+        <c:axId val="297827064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="950"/>
@@ -1900,12 +1903,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296522408"/>
+        <c:crossAx val="297862176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="296522408"/>
+        <c:axId val="297862176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1936,7 +1939,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296490040"/>
+        <c:crossAx val="297827064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2024,7 +2027,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3317,12 +3319,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="296521624"/>
-        <c:axId val="296522016"/>
-        <c:axId val="297141280"/>
+        <c:axId val="297861000"/>
+        <c:axId val="297858648"/>
+        <c:axId val="298282472"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="296521624"/>
+        <c:axId val="297861000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3359,7 +3361,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296522016"/>
+        <c:crossAx val="297858648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3367,7 +3369,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296522016"/>
+        <c:axId val="297858648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3418,12 +3420,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296521624"/>
+        <c:crossAx val="297861000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="297141280"/>
+        <c:axId val="298282472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3459,7 +3461,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296522016"/>
+        <c:crossAx val="297858648"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
       <c:spPr>
@@ -3472,7 +3474,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3689,11 +3690,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="296524760"/>
-        <c:axId val="296523584"/>
+        <c:axId val="297860216"/>
+        <c:axId val="297859824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="296524760"/>
+        <c:axId val="297860216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="950"/>
@@ -3705,12 +3706,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296523584"/>
+        <c:crossAx val="297859824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="296523584"/>
+        <c:axId val="297859824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -3722,7 +3723,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296524760"/>
+        <c:crossAx val="297860216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3810,6 +3811,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5125,11 +5127,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="296523192"/>
-        <c:axId val="296523976"/>
+        <c:axId val="297861392"/>
+        <c:axId val="297859432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="296523192"/>
+        <c:axId val="297861392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -5188,12 +5190,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296523976"/>
+        <c:crossAx val="297859432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="296523976"/>
+        <c:axId val="297859432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -5251,7 +5253,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296523192"/>
+        <c:crossAx val="297861392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5285,6 +5287,897 @@
       </c:spPr>
       <c:txPr>
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.1502352528514577E-2"/>
+          <c:y val="1.1317559185698803E-2"/>
+          <c:w val="0.95291991866684467"/>
+          <c:h val="0.94675049505287012"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Leaf:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>555</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>585</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>605</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>635</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>695</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>880</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>940</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$19:$E$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>7.55</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.549999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="315335144"/>
+        <c:axId val="315335536"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="315335144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="950"/>
+          <c:min val="450"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="315335536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="315335536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="315335144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="5000"/>
+                <a:lumOff val="95000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="76000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="45000"/>
+                <a:lumOff val="55000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="94000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="45000"/>
+                <a:lumOff val="55000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="30000"/>
+                <a:lumOff val="70000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Leaf:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>555</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>585</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>605</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>635</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7.55</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.549999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.599999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Reference</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>555</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>585</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>605</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>635</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>555</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>585</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>605</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>635</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>17.987025535795979</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.490939509136997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.659684897491534</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.90302677612733</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.726578252395129</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26.021553174727188</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.740726875540098</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>555</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>585</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>605</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>635</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$E$2:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>23.685695216958784</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.471027407533338</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.165233390621395</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.939504488279308</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.348219585972412</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.748811441032373</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.856551295788222</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="403868280"/>
+        <c:axId val="403865144"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="403868280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="403865144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="403865144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="403868280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
@@ -5382,6 +6275,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6431,6 +7364,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -6555,6 +8004,73 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>204787</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>509587</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6852,8 +8368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P79" workbookViewId="0">
-      <selection activeCell="AH19" sqref="AH19:AH27"/>
+    <sheetView topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="E18" activeCellId="1" sqref="C18:C27 E18:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9184,12 +10700,176 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>470</v>
+      </c>
+      <c r="B2" s="2">
+        <v>7.55</v>
+      </c>
+      <c r="C2">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <f>(8+(B2^2)/3+(1/B2)*90+(1/((B2*B2)*100))*10-(B2^4)/1700+(((B2^4)-5500)/10000)+(-(B2^3)/900) -0.05*B2+(B2^3)*0.0001)/2</f>
+        <v>17.987025535795979</v>
+      </c>
+      <c r="E2">
+        <f>7+((B2*(1/((A2-50)^3))*170000000)+10)-5000/A2</f>
+        <v>23.685695216958784</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>555</v>
+      </c>
+      <c r="B3" s="2">
+        <v>14.000000000000002</v>
+      </c>
+      <c r="C3">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D8" si="0">(8+(B3^2)/3+(1/B3)*90+(1/((B3*B3)*100))*10-(B3^4)/1700+(((B3^4)-5500)/10000)+(-(B3^3)/900) -0.05*B3+(B3^3)*0.0001)/2</f>
+        <v>28.490939509136997</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E8" si="1">7+((B3*(1/((A3-50)^3))*170000000)+10)-5000/A3</f>
+        <v>26.471027407533338</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>585</v>
+      </c>
+      <c r="B4" s="2">
+        <v>10.549999999999999</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>22.659684897491534</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>20.165233390621395</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>605</v>
+      </c>
+      <c r="B5" s="2">
+        <v>8.25</v>
+      </c>
+      <c r="C5">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>18.90302677612733</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>16.939504488279308</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>635</v>
+      </c>
+      <c r="B6" s="2">
+        <v>6.15</v>
+      </c>
+      <c r="C6">
+        <v>17</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>16.726578252395129</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>14.348219585972412</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>660</v>
+      </c>
+      <c r="B7" s="2">
+        <v>12.45</v>
+      </c>
+      <c r="C7">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>26.021553174727188</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>18.748811441032373</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>695</v>
+      </c>
+      <c r="B8" s="2">
+        <v>20.599999999999998</v>
+      </c>
+      <c r="C8">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>27.740726875540098</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>22.856551295788222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>880</v>
+      </c>
+      <c r="B9" s="2">
+        <v>30.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>940</v>
+      </c>
+      <c r="B10" s="2">
+        <v>20.25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>